<commit_message>
seed changes on post
</commit_message>
<xml_diff>
--- a/models/seed.xlsx
+++ b/models/seed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FF4F280-4305-4917-BE22-7007F5249B11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EEA8A52-7B8D-4FC7-97B6-374385183C47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,9 +91,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -116,13 +117,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>100012</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>61913</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1671637</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2157413</xdr:rowOff>
@@ -160,13 +161,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1428750</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1885950</xdr:rowOff>
@@ -505,68 +506,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="180.75" customHeight="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="180.75" customHeight="1">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>299</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1">
+      <c r="H1" s="2">
+        <v>43623</v>
+      </c>
+      <c r="I1" s="2">
+        <v>43623</v>
+      </c>
+      <c r="J1">
         <v>3</v>
       </c>
-      <c r="H1">
+      <c r="K1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="156.75" customHeight="1">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="156.75" customHeight="1">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>100</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="2">
+        <v>43624</v>
+      </c>
+      <c r="I2" s="2">
+        <v>43624</v>
+      </c>
+      <c r="J2">
         <v>9</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1" xr:uid="{1863CCA5-BAD2-429F-BAD7-0E5816E99C78}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{8347FFF8-73E1-4863-95B6-F838A35159B3}"/>
+    <hyperlink ref="G1" r:id="rId1" xr:uid="{1863CCA5-BAD2-429F-BAD7-0E5816E99C78}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{8347FFF8-73E1-4863-95B6-F838A35159B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>

</xml_diff>